<commit_message>
fix: correção do título
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\OneDrive\Documentos\Projetos Python\Dashboards Plotly Dash\1. People Analtics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9BAF24-9ADC-4C91-86B5-598AC964BFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="233">
   <si>
     <t>nome</t>
   </si>
@@ -704,13 +710,21 @@
   </si>
   <si>
     <t>Fernando Souza</t>
+  </si>
+  <si>
+    <t>Bruno Souza</t>
+  </si>
+  <si>
+    <t>Pablo Santos</t>
+  </si>
+  <si>
+    <t>Fernanda Santos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -767,68 +781,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -839,10 +859,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -880,71 +900,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -972,7 +992,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -995,11 +1015,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1008,13 +1028,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1024,7 +1044,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1033,7 +1053,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1042,7 +1062,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1050,10 +1070,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1118,29 +1138,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J150"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="I158" sqref="I158"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="16" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="22.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1204,7 +1223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -1234,7 +1253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1264,7 +1283,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1294,7 +1313,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1324,7 +1343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1354,7 +1373,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
@@ -1384,7 +1403,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>42</v>
       </c>
@@ -1414,7 +1433,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -1444,7 +1463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>49</v>
       </c>
@@ -1474,7 +1493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>53</v>
       </c>
@@ -1504,7 +1523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>56</v>
       </c>
@@ -1534,7 +1553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>58</v>
       </c>
@@ -1564,7 +1583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>60</v>
       </c>
@@ -1594,7 +1613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -1624,7 +1643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>65</v>
       </c>
@@ -1654,7 +1673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>67</v>
       </c>
@@ -1684,7 +1703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>69</v>
       </c>
@@ -1714,7 +1733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="33">
+    <row r="20" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>71</v>
       </c>
@@ -1744,7 +1763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>74</v>
       </c>
@@ -1774,7 +1793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>76</v>
       </c>
@@ -1804,7 +1823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>78</v>
       </c>
@@ -1834,7 +1853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>80</v>
       </c>
@@ -1864,7 +1883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>82</v>
       </c>
@@ -1894,7 +1913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="33">
+    <row r="26" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>84</v>
       </c>
@@ -1924,7 +1943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>86</v>
       </c>
@@ -1954,7 +1973,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>88</v>
       </c>
@@ -1984,7 +2003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>90</v>
       </c>
@@ -2014,7 +2033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>92</v>
       </c>
@@ -2044,7 +2063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>94</v>
       </c>
@@ -2074,7 +2093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>96</v>
       </c>
@@ -2104,7 +2123,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="33" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>97</v>
       </c>
@@ -2134,7 +2153,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="34" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>98</v>
       </c>
@@ -2166,7 +2185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="35" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>99</v>
       </c>
@@ -2196,7 +2215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="36" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>101</v>
       </c>
@@ -2228,7 +2247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="37" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>102</v>
       </c>
@@ -2258,7 +2277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="38" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>104</v>
       </c>
@@ -2290,7 +2309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="39" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>106</v>
       </c>
@@ -2320,7 +2339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="40" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>107</v>
       </c>
@@ -2350,7 +2369,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>108</v>
       </c>
@@ -2380,7 +2399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>109</v>
       </c>
@@ -2410,7 +2429,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="43" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>111</v>
       </c>
@@ -2442,7 +2461,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="44" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>112</v>
       </c>
@@ -2472,7 +2491,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="45" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>114</v>
       </c>
@@ -2502,7 +2521,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="46" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>115</v>
       </c>
@@ -2532,7 +2551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="47" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>117</v>
       </c>
@@ -2562,7 +2581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="48" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>118</v>
       </c>
@@ -2592,7 +2611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="49" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>119</v>
       </c>
@@ -2622,7 +2641,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="50" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>121</v>
       </c>
@@ -2652,7 +2671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="51" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>123</v>
       </c>
@@ -2682,7 +2701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="52" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>124</v>
       </c>
@@ -2712,7 +2731,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="53" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>126</v>
       </c>
@@ -2742,7 +2761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="54" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>127</v>
       </c>
@@ -2772,7 +2791,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="55" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>128</v>
       </c>
@@ -2802,7 +2821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="56" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>129</v>
       </c>
@@ -2832,7 +2851,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="57" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>130</v>
       </c>
@@ -2864,7 +2883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="58" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>131</v>
       </c>
@@ -2894,7 +2913,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="59" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>132</v>
       </c>
@@ -2924,7 +2943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="60" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>133</v>
       </c>
@@ -2956,7 +2975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="61" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>134</v>
       </c>
@@ -2986,7 +3005,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="62" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>136</v>
       </c>
@@ -3016,7 +3035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="63" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>138</v>
       </c>
@@ -3046,7 +3065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="64" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>139</v>
       </c>
@@ -3076,7 +3095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="65" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>140</v>
       </c>
@@ -3106,7 +3125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="66" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>141</v>
       </c>
@@ -3136,7 +3155,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="67" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>143</v>
       </c>
@@ -3166,7 +3185,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="68" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>144</v>
       </c>
@@ -3196,7 +3215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="69" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>145</v>
       </c>
@@ -3228,7 +3247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="70" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>146</v>
       </c>
@@ -3258,7 +3277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="71" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>147</v>
       </c>
@@ -3288,7 +3307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="72" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>148</v>
       </c>
@@ -3318,7 +3337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="73" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>149</v>
       </c>
@@ -3348,7 +3367,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="74" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>151</v>
       </c>
@@ -3378,7 +3397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="75" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>152</v>
       </c>
@@ -3408,7 +3427,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="76" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>153</v>
       </c>
@@ -3438,7 +3457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="77" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>154</v>
       </c>
@@ -3468,7 +3487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="78" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>155</v>
       </c>
@@ -3498,7 +3517,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="79" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>156</v>
       </c>
@@ -3528,7 +3547,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="80" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>157</v>
       </c>
@@ -3558,7 +3577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="81" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>158</v>
       </c>
@@ -3588,7 +3607,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="82" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>159</v>
       </c>
@@ -3618,7 +3637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="83" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>161</v>
       </c>
@@ -3648,7 +3667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="84" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>163</v>
       </c>
@@ -3678,7 +3697,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="85" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>164</v>
       </c>
@@ -3708,7 +3727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="86" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>165</v>
       </c>
@@ -3738,7 +3757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="87" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>166</v>
       </c>
@@ -3768,7 +3787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="88" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>167</v>
       </c>
@@ -3798,7 +3817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="89" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>169</v>
       </c>
@@ -3828,7 +3847,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="90" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>170</v>
       </c>
@@ -3858,7 +3877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="91" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>171</v>
       </c>
@@ -3888,7 +3907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="92" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>172</v>
       </c>
@@ -3918,7 +3937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="93" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>173</v>
       </c>
@@ -3948,7 +3967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="94" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>174</v>
       </c>
@@ -3978,7 +3997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="95" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>175</v>
       </c>
@@ -4008,7 +4027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="96" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>176</v>
       </c>
@@ -4038,7 +4057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="97" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>177</v>
       </c>
@@ -4068,7 +4087,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="98" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>178</v>
       </c>
@@ -4098,7 +4117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="99" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>179</v>
       </c>
@@ -4128,7 +4147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="100" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>180</v>
       </c>
@@ -4158,7 +4177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="101" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>181</v>
       </c>
@@ -4188,7 +4207,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="102" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>182</v>
       </c>
@@ -4218,7 +4237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="103" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>183</v>
       </c>
@@ -4248,7 +4267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="104" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>184</v>
       </c>
@@ -4278,7 +4297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="105" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>185</v>
       </c>
@@ -4308,7 +4327,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="106" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>186</v>
       </c>
@@ -4338,7 +4357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="107" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>187</v>
       </c>
@@ -4368,7 +4387,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="108" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>111</v>
       </c>
@@ -4398,7 +4417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="109" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>188</v>
       </c>
@@ -4428,7 +4447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="110" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>189</v>
       </c>
@@ -4458,7 +4477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="111" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>190</v>
       </c>
@@ -4488,7 +4507,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="112" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>191</v>
       </c>
@@ -4518,7 +4537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="113" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>192</v>
       </c>
@@ -4548,7 +4567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="114" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>193</v>
       </c>
@@ -4578,7 +4597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="115" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>194</v>
       </c>
@@ -4608,7 +4627,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="116" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>195</v>
       </c>
@@ -4638,7 +4657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="117" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>196</v>
       </c>
@@ -4668,7 +4687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="118" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>197</v>
       </c>
@@ -4698,7 +4717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="119" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>198</v>
       </c>
@@ -4728,7 +4747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="120" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>199</v>
       </c>
@@ -4758,7 +4777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="121" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>200</v>
       </c>
@@ -4788,7 +4807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="122" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>201</v>
       </c>
@@ -4818,7 +4837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="123" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>202</v>
       </c>
@@ -4848,7 +4867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="124" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>203</v>
       </c>
@@ -4878,7 +4897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="125" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>204</v>
       </c>
@@ -4908,7 +4927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="126" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>205</v>
       </c>
@@ -4938,7 +4957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="127" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>206</v>
       </c>
@@ -4968,7 +4987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="128" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>207</v>
       </c>
@@ -4998,7 +5017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="129" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>208</v>
       </c>
@@ -5028,7 +5047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="130" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>209</v>
       </c>
@@ -5058,7 +5077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="131" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>210</v>
       </c>
@@ -5088,7 +5107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="132" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>211</v>
       </c>
@@ -5118,7 +5137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="133" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>212</v>
       </c>
@@ -5148,7 +5167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="134" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>213</v>
       </c>
@@ -5180,7 +5199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="135" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>214</v>
       </c>
@@ -5210,7 +5229,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="136" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>215</v>
       </c>
@@ -5240,7 +5259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="137" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>216</v>
       </c>
@@ -5270,7 +5289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="138" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>217</v>
       </c>
@@ -5300,7 +5319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="139" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>218</v>
       </c>
@@ -5330,7 +5349,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="140" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>219</v>
       </c>
@@ -5360,7 +5379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="141" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>221</v>
       </c>
@@ -5390,7 +5409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="142" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>222</v>
       </c>
@@ -5420,7 +5439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="143" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>223</v>
       </c>
@@ -5450,7 +5469,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="144" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>224</v>
       </c>
@@ -5480,7 +5499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="145" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>225</v>
       </c>
@@ -5510,7 +5529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="146" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>226</v>
       </c>
@@ -5540,7 +5559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="147" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>227</v>
       </c>
@@ -5570,7 +5589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="148" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>78</v>
       </c>
@@ -5602,7 +5621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="149" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>228</v>
       </c>
@@ -5634,7 +5653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="150" spans="1:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>229</v>
       </c>
@@ -5661,6 +5680,96 @@
         <v>62</v>
       </c>
       <c r="J150" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B151" s="7">
+        <v>3000</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F151" s="8">
+        <v>44578</v>
+      </c>
+      <c r="G151" s="8"/>
+      <c r="H151" s="9">
+        <v>70</v>
+      </c>
+      <c r="I151" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J151" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B152" s="7">
+        <v>3500</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F152" s="8">
+        <v>44676</v>
+      </c>
+      <c r="G152" s="8"/>
+      <c r="H152" s="9">
+        <v>86</v>
+      </c>
+      <c r="I152" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J152" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B153" s="7">
+        <v>8300</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" s="8">
+        <v>44632</v>
+      </c>
+      <c r="G153" s="8"/>
+      <c r="H153" s="9">
+        <v>89</v>
+      </c>
+      <c r="I153" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J153" s="6" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>